<commit_message>
add malware 2010-2017 installation results
</commit_message>
<xml_diff>
--- a/Data/Bar(completed)-Malware.xlsx
+++ b/Data/Bar(completed)-Malware.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxiang\Desktop\REU-Android-Spring2022\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE1B4C7-DD61-4214-AB3A-B292A03703FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F2379A-5D8C-467E-BD5D-359775D67AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="install" sheetId="1" r:id="rId1"/>
     <sheet name="run" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>DELETE_FAILED_INTERNAL_ERROR</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -163,6 +166,21 @@
   <si>
     <t>malware-2017</t>
   </si>
+  <si>
+    <t>INSTALL_FAILED_PERMISSION_MODEL_DOWNGRADE</t>
+  </si>
+  <si>
+    <t>INSTALL_FAILED_SHARED_USER_INCOMPATIBLE</t>
+  </si>
+  <si>
+    <t>INSTALL_PARSE_FAILED_INCONSISTENT_CERTIFICATES</t>
+  </si>
+  <si>
+    <t>INSTALL_FAILED_DEXOPT</t>
+  </si>
+  <si>
+    <t>INSTALL_FAILED_MEDIA_UNAVAILABLE</t>
+  </si>
 </sst>
 </file>
 
@@ -172,7 +190,7 @@
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
     <numFmt numFmtId="165" formatCode="0.000000_);[Red]\(0.000000\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +213,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -217,12 +236,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -246,6 +267,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -285,7 +319,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -300,10 +334,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -343,17 +393,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.3494418577789272E-2"/>
-          <c:y val="5.8432983809002359E-2"/>
-          <c:w val="0.49911514038122529"/>
-          <c:h val="0.76068660638211993"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
@@ -384,13 +424,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -398,14 +462,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$2:$C$2</c:f>
+              <c:f>install!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1.5641493138854198E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>1.0257111597374099E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -413,7 +495,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000000-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -443,13 +525,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -457,14 +563,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$3:$C$3</c:f>
+              <c:f>install!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.782178217821782E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.5143043620145765E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8544243577545197E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3169984686064313E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.916452221650369E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6794419085350099E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2038567493112946E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -472,7 +602,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000001-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -502,13 +632,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -516,14 +670,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$4:$C$4</c:f>
+              <c:f>install!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9.1101925378005003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1883614088820824E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7155601303825698E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4382912755145982E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -531,7 +706,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000002-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -561,13 +736,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -575,14 +774,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$5:$C$5</c:f>
+              <c:f>install!$B$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000_);[Red]\(0.0000\)">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -590,7 +807,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000003-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -620,13 +837,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -634,14 +875,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$6:$C$6</c:f>
+              <c:f>install!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.3861386138613862E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9580115305123462E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1417697431018079E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30333078101071975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35825184422714018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4938420463353713E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1068870523415978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1594202898550725E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.73879666058919402</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>0.50041028446389502</c:v>
                 </c:pt>
               </c:numCache>
@@ -649,7 +914,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000004-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -668,14 +933,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="dkUpDiag">
-              <a:fgClr>
-                <a:srgbClr val="00B050"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -684,13 +944,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -698,14 +982,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$7:$C$7</c:f>
+              <c:f>install!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0" formatCode="0.00E+00">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30792079207920792</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.82747742847819E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1417697431018079E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2542113323124044E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0066906845084926E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1340108517784859E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2855831037649219E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0434782608695653E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
                   <c:v>9.5960080606467704E-5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -713,7 +1021,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000005-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -732,14 +1040,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="dkDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,13 +1053,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -762,14 +1091,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$8:$C$8</c:f>
+              <c:f>install!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80365495485695637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97954329210275926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5746554364471669E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26265225596157143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7167771940401344</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74986225895316805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91884057971014488</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.23586987813069701</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>0.44666301969365402</c:v>
                 </c:pt>
               </c:numCache>
@@ -777,7 +1130,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000006-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -809,13 +1162,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -823,14 +1200,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$9:$C$9</c:f>
+              <c:f>install!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8985507246376812E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5.5656846751751202E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>2.2839168490153099E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -838,7 +1233,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000007-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -851,7 +1246,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_FAILED_VERSION_DOWNGRADE</c:v>
+                  <c:v>INSTALL_FAILED_PERMISSION_MODEL_DOWNGRADE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -870,13 +1265,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -884,14 +1303,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$10:$C$10</c:f>
+              <c:f>install!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>9.5960080606467704E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3062613039359228E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -899,7 +1327,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000008-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -912,7 +1340,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_BAD_MANIFEST</c:v>
+                  <c:v>INSTALL_FAILED_SHARED_USER_INCOMPATIBLE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -931,13 +1359,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -945,14 +1397,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$11:$C$11</c:f>
+              <c:f>install!$B$11:$K$11</c:f>
               <c:numCache>
-                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1444501629782123E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -960,7 +1421,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{00000009-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -973,7 +1434,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_BAD_PACKAGE_NAME</c:v>
+                  <c:v>INSTALL_FAILED_VERSION_DOWNGRADE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -992,13 +1453,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1006,14 +1491,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$12:$C$12</c:f>
+              <c:f>install!$B$12:$K$12</c:f>
               <c:numCache>
-                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.401946430109379E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.6932966023875119E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>9.5960080606467704E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1021,7 +1524,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000A-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1034,7 +1537,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_BAD_SHARED_USER_ID</c:v>
+                  <c:v>INSTALL_PARSE_FAILED_BAD_MANIFEST</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1053,13 +1556,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1067,14 +1594,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$13:$C$13</c:f>
+              <c:f>install!$B$13:$K$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7088487155090395E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3062613039359228E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000_);[Red]\(0.0000\)">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1082,7 +1630,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000B-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1095,7 +1643,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_MANIFEST_MALFORMED</c:v>
+                  <c:v>INSTALL_PARSE_FAILED_BAD_PACKAGE_NAME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1115,13 +1663,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1129,14 +1701,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$14:$C$14</c:f>
+              <c:f>install!$B$14:$K$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000_);[Red]\(0.0000\)">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1144,7 +1734,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000C-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1157,7 +1747,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_NO_CERTIFICATES</c:v>
+                  <c:v>INSTALL_PARSE_FAILED_BAD_SHARED_USER_ID</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1177,13 +1767,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1191,22 +1805,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$15:$C$15</c:f>
+              <c:f>install!$B$15:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2.87880241819403E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.36761487964989E-4</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000D-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1219,7 +1851,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>INSTALL_PARSE_FAILED_UNEXPECTED_EXCEPTION</c:v>
+                  <c:v>INSTALL_PARSE_FAILED_MANIFEST_MALFORMED</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1239,13 +1871,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1253,22 +1909,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$16:$C$16</c:f>
+              <c:f>install!$B$16:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2.1111217733422801E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9146608315098401E-2</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.8811881188118811E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1485451761102603E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2866700977869275E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0143829127551462E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3461891643709823E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000_);[Red]\(0.0000\)">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000E-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1281,14 +1955,17 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NO MESSAGE</c:v>
+                  <c:v>INSTALL_PARSE_FAILED_NO_CERTIFICATES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1298,13 +1975,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>install!$B$1:$C$1</c:f>
+              <c:f>install!$B$1:$K$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>malware-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>malware-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -1312,22 +2013,548 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>install!$B$17:$C$17</c:f>
+              <c:f>install!$B$17:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.53536128970348E-3</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.9603960396039604E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.47045951859956E-4</c:v>
+                  <c:v>7.6144892853257913E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5459418070444104E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.56201749871333E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2315907329256739E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4416896235078053E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.87880241819403E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.36761487964989E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-5BA8-473E-BDF8-C44FB2E75C3E}"/>
+              <c16:uniqueId val="{0000000F-9C9D-496D-A96B-48491EEB73E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>install!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>INSTALL_PARSE_FAILED_UNEXPECTED_EXCEPTION</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>install!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>malware-2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>malware-2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>install!$B$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.22277227722772278</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.158381377134776E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3787519142419602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35786584319780407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3258978554818712E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10587695133149679</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1594202898550725E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1111217733422801E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9146608315098401E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-9C9D-496D-A96B-48491EEB73E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>install!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO MESSAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>install!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>malware-2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>malware-2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>install!$B$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.4851485148514851E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6425541172631349E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6460513796384395E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23746171516079634</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0924686910276199E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10623546636809922</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2396694214876033E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4637681159420291E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.53536128970348E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.47045951859956E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-9C9D-496D-A96B-48491EEB73E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>install!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>INSTALL_PARSE_FAILED_INCONSISTENT_CERTIFICATES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>install!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>malware-2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>malware-2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>install!$B$20:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.577800651912849E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5837567823615537E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6730945821854911E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-9C9D-496D-A96B-48491EEB73E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>install!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>INSTALL_FAILED_DEXOPT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>install!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>malware-2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>malware-2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>install!$B$21:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>6.249320134885239E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5632730732635581E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1485451761102603E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1580030880082347E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2967014038411853E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7548209366391182E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-9C9D-496D-A96B-48491EEB73E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>install!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>INSTALL_FAILED_MEDIA_UNAVAILABLE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>install!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>malware-2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>malware-2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>malware-2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>malware-2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>malware-2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>malware-2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>malware-2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>malware-2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>malware-2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>malware-2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>install!$B$22:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>5.7427258805513015E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9330806993368362E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-9C9D-496D-A96B-48491EEB73E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1341,11 +2568,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="251292544"/>
-        <c:axId val="340490144"/>
+        <c:axId val="55942832"/>
+        <c:axId val="55940752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251292544"/>
+        <c:axId val="55942832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +2596,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="960000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1380,7 +2607,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1388,7 +2615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340490144"/>
+        <c:crossAx val="55940752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1396,7 +2623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340490144"/>
+        <c:axId val="55940752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,7 +2666,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1447,7 +2674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251292544"/>
+        <c:crossAx val="55942832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,17 +2687,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.58968204142390657"/>
-          <c:y val="1.0140008158804203E-2"/>
-          <c:w val="0.33785940194298303"/>
-          <c:h val="0.89159412258218451"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1491,7 +2708,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
+              <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1502,13 +2719,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1531,9 +2741,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
-        </a:defRPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1541,7 +2749,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup paperSize="9" orientation="landscape"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4064,23 +5272,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1833559</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>386952</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>182163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>952499</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE52A97D-A92E-44BB-ABD9-A2FEA870303B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8D8516-49F4-47F5-D92D-104B9C041CE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4140,6 +5348,512 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="install"/>
+      <sheetName val="run"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>benign-2010</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>benign-2011</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>benign-2012</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>benign-2013</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>benign-2014</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>benign-2015</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>benign-2016</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>benign-2017</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>DELETE_FAILED_INTERNAL_ERROR</v>
+          </cell>
+          <cell r="B2">
+            <v>3.5500000000000002E-3</v>
+          </cell>
+          <cell r="C2">
+            <v>9.7000000000000005E-4</v>
+          </cell>
+          <cell r="D2">
+            <v>2.9334220000000002E-3</v>
+          </cell>
+          <cell r="E2">
+            <v>7.6611300000000002E-4</v>
+          </cell>
+          <cell r="F2">
+            <v>2.2499999999999998E-3</v>
+          </cell>
+          <cell r="G2">
+            <v>3.6099999999999999E-3</v>
+          </cell>
+          <cell r="H2">
+            <v>2.82E-3</v>
+          </cell>
+          <cell r="I2">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>INSTALL_FAILED_DUPLICATE_PERMISSION</v>
+          </cell>
+          <cell r="B3">
+            <v>0</v>
+          </cell>
+          <cell r="C3">
+            <v>0</v>
+          </cell>
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3">
+            <v>5.3888600000000003E-4</v>
+          </cell>
+          <cell r="F3">
+            <v>0</v>
+          </cell>
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+          <cell r="H3">
+            <v>0</v>
+          </cell>
+          <cell r="I3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>INSTALL_FAILED_INSUFFICIENT_STORAGE</v>
+          </cell>
+          <cell r="B4">
+            <v>0</v>
+          </cell>
+          <cell r="C4">
+            <v>0</v>
+          </cell>
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+          <cell r="E4">
+            <v>0</v>
+          </cell>
+          <cell r="F4">
+            <v>1.2999999999999999E-4</v>
+          </cell>
+          <cell r="G4">
+            <v>2.9999999999999997E-4</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+          <cell r="I4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>INSTALL_FAILED_INTERNAL_ERROR</v>
+          </cell>
+          <cell r="B5">
+            <v>0</v>
+          </cell>
+          <cell r="C5">
+            <v>0</v>
+          </cell>
+          <cell r="D5">
+            <v>0</v>
+          </cell>
+          <cell r="E5">
+            <v>0</v>
+          </cell>
+          <cell r="F5">
+            <v>9.3000000000000005E-4</v>
+          </cell>
+          <cell r="G5">
+            <v>5.5199999999999997E-3</v>
+          </cell>
+          <cell r="H5">
+            <v>0</v>
+          </cell>
+          <cell r="I5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>INSTALL_FAILED_INVALID_APK</v>
+          </cell>
+          <cell r="B6">
+            <v>3.3500000000000001E-3</v>
+          </cell>
+          <cell r="C6">
+            <v>7.2999999999999996E-4</v>
+          </cell>
+          <cell r="D6">
+            <v>1.5527679999999999E-3</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>2.1299999999999999E-3</v>
+          </cell>
+          <cell r="G6">
+            <v>6.0999999999999997E-4</v>
+          </cell>
+          <cell r="H6">
+            <v>0</v>
+          </cell>
+          <cell r="I6">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>INSTALL_FAILED_MISSING_SHARED_LIBRARY</v>
+          </cell>
+          <cell r="B7">
+            <v>1.1100000000000001E-3</v>
+          </cell>
+          <cell r="C7">
+            <v>1.2930000000000001E-2</v>
+          </cell>
+          <cell r="D7">
+            <v>7.1798369999999997E-3</v>
+          </cell>
+          <cell r="E7">
+            <v>7.5335690000000004E-3</v>
+          </cell>
+          <cell r="F7">
+            <v>1.235E-2</v>
+          </cell>
+          <cell r="G7">
+            <v>2.14E-3</v>
+          </cell>
+          <cell r="H7">
+            <v>0.15343999999999999</v>
+          </cell>
+          <cell r="I7">
+            <v>0.15034</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>INSTALL_FAILED_NO_MATCHING_ABIS</v>
+          </cell>
+          <cell r="B8">
+            <v>0.95721000000000001</v>
+          </cell>
+          <cell r="C8">
+            <v>0.96135000000000004</v>
+          </cell>
+          <cell r="D8">
+            <v>0.97553486199999995</v>
+          </cell>
+          <cell r="E8">
+            <v>0.96880630199999995</v>
+          </cell>
+          <cell r="F8">
+            <v>0.94860999999999995</v>
+          </cell>
+          <cell r="G8">
+            <v>0.95343</v>
+          </cell>
+          <cell r="H8">
+            <v>0.78434999999999999</v>
+          </cell>
+          <cell r="I8">
+            <v>0.77975000000000005</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>INSTALL_FAILED_OLDER_SDK</v>
+          </cell>
+          <cell r="B9">
+            <v>8.5999999999999998E-4</v>
+          </cell>
+          <cell r="C9">
+            <v>0</v>
+          </cell>
+          <cell r="D9">
+            <v>0</v>
+          </cell>
+          <cell r="E9">
+            <v>0</v>
+          </cell>
+          <cell r="F9">
+            <v>9.3000000000000005E-4</v>
+          </cell>
+          <cell r="G9">
+            <v>0</v>
+          </cell>
+          <cell r="H9">
+            <v>0</v>
+          </cell>
+          <cell r="I9">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>INSTALL_FAILED_VERSION_DOWNGRADE</v>
+          </cell>
+          <cell r="B12">
+            <v>3.6999999999999999E-4</v>
+          </cell>
+          <cell r="C12">
+            <v>0</v>
+          </cell>
+          <cell r="D12">
+            <v>0</v>
+          </cell>
+          <cell r="E12">
+            <v>0</v>
+          </cell>
+          <cell r="F12">
+            <v>0</v>
+          </cell>
+          <cell r="G12">
+            <v>0</v>
+          </cell>
+          <cell r="H12">
+            <v>0</v>
+          </cell>
+          <cell r="I12">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>INSTALL_PARSE_FAILED_BAD_MANIFEST</v>
+          </cell>
+          <cell r="B13">
+            <v>0</v>
+          </cell>
+          <cell r="C13">
+            <v>0</v>
+          </cell>
+          <cell r="D13">
+            <v>0</v>
+          </cell>
+          <cell r="E13">
+            <v>0</v>
+          </cell>
+          <cell r="F13">
+            <v>0</v>
+          </cell>
+          <cell r="G13">
+            <v>1.4999999999999999E-4</v>
+          </cell>
+          <cell r="H13">
+            <v>0</v>
+          </cell>
+          <cell r="I13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>INSTALL_PARSE_FAILED_BAD_PACKAGE_NAME</v>
+          </cell>
+          <cell r="B14">
+            <v>1.47E-3</v>
+          </cell>
+          <cell r="C14">
+            <v>0</v>
+          </cell>
+          <cell r="D14">
+            <v>2.5313400000000002E-4</v>
+          </cell>
+          <cell r="E14">
+            <v>0</v>
+          </cell>
+          <cell r="F14">
+            <v>0</v>
+          </cell>
+          <cell r="G14">
+            <v>0</v>
+          </cell>
+          <cell r="H14">
+            <v>0</v>
+          </cell>
+          <cell r="I14">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>INSTALL_PARSE_FAILED_BAD_SHARED_USER_ID</v>
+          </cell>
+          <cell r="B15">
+            <v>5.1799999999999997E-3</v>
+          </cell>
+          <cell r="C15">
+            <v>0</v>
+          </cell>
+          <cell r="D15">
+            <v>0</v>
+          </cell>
+          <cell r="E15">
+            <v>0</v>
+          </cell>
+          <cell r="F15">
+            <v>0</v>
+          </cell>
+          <cell r="G15">
+            <v>0</v>
+          </cell>
+          <cell r="H15">
+            <v>0</v>
+          </cell>
+          <cell r="I15">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>INSTALL_PARSE_FAILED_MANIFEST_MALFORMED</v>
+          </cell>
+          <cell r="B16">
+            <v>8.5999999999999998E-4</v>
+          </cell>
+          <cell r="C16">
+            <v>0</v>
+          </cell>
+          <cell r="D16">
+            <v>0</v>
+          </cell>
+          <cell r="E16">
+            <v>0</v>
+          </cell>
+          <cell r="F16">
+            <v>2.5999999999999998E-4</v>
+          </cell>
+          <cell r="G16">
+            <v>2.3900000000000002E-3</v>
+          </cell>
+          <cell r="H16">
+            <v>0</v>
+          </cell>
+          <cell r="I16">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>INSTALL_PARSE_FAILED_NO_CERTIFICATES</v>
+          </cell>
+          <cell r="B17">
+            <v>2.3400000000000001E-3</v>
+          </cell>
+          <cell r="C17">
+            <v>2.5000000000000001E-4</v>
+          </cell>
+          <cell r="D17">
+            <v>0</v>
+          </cell>
+          <cell r="E17">
+            <v>1.54528E-4</v>
+          </cell>
+          <cell r="F17">
+            <v>1.73E-3</v>
+          </cell>
+          <cell r="G17">
+            <v>1.5200000000000001E-3</v>
+          </cell>
+          <cell r="H17">
+            <v>0</v>
+          </cell>
+          <cell r="I17">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>INSTALL_PARSE_FAILED_UNEXPECTED_EXCEPTION</v>
+          </cell>
+          <cell r="B18">
+            <v>3.0699999999999998E-3</v>
+          </cell>
+          <cell r="C18">
+            <v>9.7999999999999997E-4</v>
+          </cell>
+          <cell r="D18">
+            <v>1.265668E-3</v>
+          </cell>
+          <cell r="E18">
+            <v>4.3110830000000003E-3</v>
+          </cell>
+          <cell r="F18">
+            <v>4.9199999999999999E-3</v>
+          </cell>
+          <cell r="G18">
+            <v>1.3699999999999999E-3</v>
+          </cell>
+          <cell r="H18">
+            <v>2.513E-2</v>
+          </cell>
+          <cell r="I18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>NO MESSAGE</v>
+          </cell>
+          <cell r="B19">
+            <v>2.0619999999999999E-2</v>
+          </cell>
+          <cell r="C19">
+            <v>2.2800000000000001E-2</v>
+          </cell>
+          <cell r="D19">
+            <v>1.0520909E-2</v>
+          </cell>
+          <cell r="E19">
+            <v>1.7889519E-2</v>
+          </cell>
+          <cell r="F19">
+            <v>2.5770000000000001E-2</v>
+          </cell>
+          <cell r="G19">
+            <v>2.895E-2</v>
+          </cell>
+          <cell r="H19">
+            <v>3.4270000000000002E-2</v>
+          </cell>
+          <cell r="I19">
+            <v>6.991E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4405,223 +6119,784 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="2"/>
+    <col min="2" max="2" width="15.75" style="8" customWidth="1"/>
+    <col min="3" max="6" width="14.125" style="8" customWidth="1"/>
+    <col min="7" max="9" width="15" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="15">
+        <f>0/111</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16">
         <v>1.5641493138854198E-2</v>
       </c>
-      <c r="C2">
+      <c r="K2" s="16">
         <v>1.0257111597374099E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="17">
+        <f>18/1010</f>
+        <v>1.782178217821782E-2</v>
+      </c>
+      <c r="C3" s="17">
+        <f>83/18386</f>
+        <v>4.5143043620145765E-3</v>
+      </c>
+      <c r="D3" s="17">
+        <f>3/10510</f>
+        <v>2.8544243577545197E-4</v>
+      </c>
+      <c r="E3" s="17">
+        <v>6.3169984686064313E-4</v>
+      </c>
+      <c r="F3" s="17">
+        <v>2.916452221650369E-3</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1.6794419085350099E-3</v>
+      </c>
+      <c r="H3" s="17">
+        <v>2.2038567493112946E-3</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="16">
+        <v>0</v>
+      </c>
+      <c r="K3" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="17">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17">
+        <f>1675/18386</f>
+        <v>9.1101925378005003E-2</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17">
+        <v>9.1883614088820824E-4</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1.7155601303825698E-4</v>
+      </c>
+      <c r="G4" s="17">
+        <v>1.4382912755145982E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16">
+        <v>0</v>
+      </c>
+      <c r="K4" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="17">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
+        <f>14/1010</f>
+        <v>1.3861386138613862E-2</v>
+      </c>
+      <c r="C6" s="15">
+        <f>36/18386</f>
+        <v>1.9580115305123462E-3</v>
+      </c>
+      <c r="D6" s="15">
+        <f>12/10510</f>
+        <v>1.1417697431018079E-3</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.30333078101071975</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.35825184422714018</v>
+      </c>
+      <c r="G6" s="15">
+        <v>6.4938420463353713E-2</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.1068870523415978</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.1594202898550725E-2</v>
+      </c>
+      <c r="J6" s="16">
         <v>0.73879666058919402</v>
       </c>
-      <c r="C6">
+      <c r="K6" s="16">
         <v>0.50041028446389502</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="15">
+        <f>311/1010</f>
+        <v>0.30792079207920792</v>
+      </c>
+      <c r="C7" s="15">
+        <f>336/18386</f>
+        <v>1.82747742847819E-2</v>
+      </c>
+      <c r="D7" s="15">
+        <f>12/10510</f>
+        <v>1.1417697431018079E-3</v>
+      </c>
+      <c r="E7" s="15">
+        <v>3.2542113323124044E-4</v>
+      </c>
+      <c r="F7" s="15">
+        <v>9.0066906845084926E-4</v>
+      </c>
+      <c r="G7" s="15">
+        <v>4.1340108517784859E-3</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1.2855831037649219E-3</v>
+      </c>
+      <c r="I7" s="15">
+        <v>3.0434782608695653E-2</v>
+      </c>
+      <c r="J7" s="19">
         <v>9.5960080606467704E-5</v>
       </c>
-      <c r="C7">
+      <c r="K7" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="15">
+        <f>404/1010</f>
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="15">
+        <f>14776/18386</f>
+        <v>0.80365495485695637</v>
+      </c>
+      <c r="D8" s="15">
+        <f>10295/10510</f>
+        <v>0.97954329210275926</v>
+      </c>
+      <c r="E8" s="15">
+        <v>7.5746554364471669E-2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.26265225596157143</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.7167771940401344</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0.74986225895316805</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0.91884057971014488</v>
+      </c>
+      <c r="J8" s="16">
         <v>0.23586987813069701</v>
       </c>
-      <c r="C8">
+      <c r="K8" s="16">
         <v>0.44666301969365402</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="17">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>2.8985507246376812E-3</v>
+      </c>
+      <c r="J9" s="16">
         <v>5.5656846751751202E-3</v>
       </c>
-      <c r="C9">
+      <c r="K9" s="16">
         <v>2.2839168490153099E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17">
+        <v>0</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>4.3062613039359228E-5</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2.1444501629782123E-4</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B12" s="15">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>3.401946430109379E-3</v>
+      </c>
+      <c r="H12" s="15">
+        <v>5.6932966023875119E-3</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0</v>
+      </c>
+      <c r="J12" s="19">
         <v>9.5960080606467704E-5</v>
       </c>
-      <c r="C10">
+      <c r="K12" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15">
+        <f>6/10510</f>
+        <v>5.7088487155090395E-4</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>4.3062613039359228E-5</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15">
+        <v>0</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+      <c r="H14" s="15">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B15" s="17">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17">
+        <v>0</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B16" s="15">
+        <f>19/1010</f>
+        <v>1.8811881188118811E-2</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15">
+        <v>1.1485451761102603E-4</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1.2866700977869275E-4</v>
+      </c>
+      <c r="G16" s="15">
+        <v>3.0143829127551462E-4</v>
+      </c>
+      <c r="H16" s="15">
+        <v>7.3461891643709823E-4</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
+        <v>0</v>
+      </c>
+      <c r="K16" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B17" s="15">
+        <f>4/1010</f>
+        <v>3.9603960396039604E-3</v>
+      </c>
+      <c r="C17" s="15">
+        <f>14/18386</f>
+        <v>7.6144892853257913E-4</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15">
+        <v>2.5459418070444104E-3</v>
+      </c>
+      <c r="F17" s="15">
+        <v>6.56201749871333E-3</v>
+      </c>
+      <c r="G17" s="15">
+        <v>1.2315907329256739E-2</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1.4416896235078053E-2</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
         <v>2.87880241819403E-4</v>
       </c>
-      <c r="C15">
+      <c r="K17" s="16">
         <v>1.36761487964989E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B18" s="15">
+        <f>225/1010</f>
+        <v>0.22277227722772278</v>
+      </c>
+      <c r="C18" s="15">
+        <f>15/18386</f>
+        <v>8.158381377134776E-4</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15">
+        <v>0.3787519142419602</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0.35786584319780407</v>
+      </c>
+      <c r="G18" s="15">
+        <v>6.3258978554818712E-2</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0.10587695133149679</v>
+      </c>
+      <c r="I18" s="15">
+        <v>1.1594202898550725E-2</v>
+      </c>
+      <c r="J18" s="16">
         <v>2.1111217733422801E-3</v>
       </c>
-      <c r="C16">
+      <c r="K18" s="16">
         <v>1.9146608315098401E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B19" s="15">
+        <f>15/1010</f>
+        <v>1.4851485148514851E-2</v>
+      </c>
+      <c r="C19" s="15">
+        <f>302/18386</f>
+        <v>1.6425541172631349E-2</v>
+      </c>
+      <c r="D19" s="15">
+        <f>173/10510</f>
+        <v>1.6460513796384395E-2</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.23746171516079634</v>
+      </c>
+      <c r="F19" s="15">
+        <v>9.0924686910276199E-3</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0.10623546636809922</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1.2396694214876033E-2</v>
+      </c>
+      <c r="I19" s="15">
+        <v>2.4637681159420291E-2</v>
+      </c>
+      <c r="J19" s="16">
         <v>1.53536128970348E-3</v>
       </c>
-      <c r="C17">
+      <c r="K19" s="16">
         <v>5.47045951859956E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="F20" s="15">
+        <v>8.577800651912849E-5</v>
+      </c>
+      <c r="G20" s="15">
+        <v>2.5837567823615537E-4</v>
+      </c>
+      <c r="H20" s="15">
+        <v>3.6730945821854911E-4</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15">
+        <f>1149/18386</f>
+        <v>6.249320134885239E-2</v>
+      </c>
+      <c r="D21" s="15">
+        <f>9/10510</f>
+        <v>8.5632730732635581E-4</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1.1485451761102603E-4</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1.1580030880082347E-3</v>
+      </c>
+      <c r="G21" s="15">
+        <v>5.2967014038411853E-3</v>
+      </c>
+      <c r="H21" s="15">
+        <v>2.7548209366391182E-4</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15">
+        <v>5.7427258805513015E-5</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>6.9330806993368362E-3</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="12">
-        <f>SUM(B2:B17)</f>
+      <c r="B23" s="17">
+        <f>SUM(B2:B22)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="17">
+        <f>SUM(C2:C22)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="17">
+        <f>SUM(D2:D22)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E23" s="17">
+        <f>SUM(E2:E22)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="17">
+        <f>SUM(F2:F22)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="17">
+        <f>SUM(G2:G22)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H23" s="17">
+        <f>SUM(H2:H22)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I23" s="17">
+        <f>SUM(I2:I22)</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="18">
+        <f>SUM(J2:J19)</f>
         <v>0.99999999999999833</v>
       </c>
-      <c r="C18" s="12">
-        <f>SUM(C2:C17)</f>
+      <c r="K23" s="18">
+        <f>SUM(K2:K19)</f>
         <v>0.99999999999999967</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4629,8 +6904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4703,10 +6978,10 @@
       <c r="G2" s="3">
         <v>1.9430051813471499E-2</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="13">
         <v>3.3222591362126199E-3</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <v>3.9968025579536299E-4</v>
       </c>
       <c r="J2" s="2">
@@ -4738,10 +7013,10 @@
       <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="15">
-        <v>0</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
         <v>0</v>
       </c>
       <c r="J3" s="3">
@@ -4773,10 +7048,10 @@
       <c r="G4" s="3">
         <v>3.8860103626943E-3</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>3.3222591362126199E-3</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>3.9968025579536299E-4</v>
       </c>
       <c r="J4" s="2">
@@ -4808,10 +7083,10 @@
       <c r="G5" s="3">
         <v>0.21243523316062099</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="13">
         <v>9.8837209302325493E-2</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <v>4.23661071143085E-2</v>
       </c>
       <c r="J5" s="2">
@@ -4825,7 +7100,7 @@
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>0</v>
       </c>
       <c r="C6" s="3">
@@ -4834,7 +7109,7 @@
       <c r="D6" s="3">
         <v>9.5652173913043398E-2</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>0</v>
       </c>
       <c r="F6" s="3">
@@ -4843,10 +7118,10 @@
       <c r="G6" s="3">
         <v>0.142487046632124</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="13">
         <v>0.111295681063122</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <v>0.105915267785771</v>
       </c>
       <c r="J6" s="2">
@@ -4860,7 +7135,7 @@
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>0</v>
       </c>
       <c r="C7" s="3">
@@ -4878,10 +7153,10 @@
       <c r="G7" s="3">
         <v>1.2953367875647599E-3</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <v>6.6445182724252398E-3</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <v>1.07913669064748E-2</v>
       </c>
       <c r="J7" s="2">
@@ -4895,7 +7170,7 @@
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>0</v>
       </c>
       <c r="C8" s="3">
@@ -4913,10 +7188,10 @@
       <c r="G8" s="3">
         <v>0</v>
       </c>
-      <c r="H8" s="15">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
         <v>0</v>
       </c>
       <c r="J8" s="3">
@@ -4948,10 +7223,10 @@
       <c r="G9" s="3">
         <v>4.92227979274611E-2</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="13">
         <v>3.32225913621262E-2</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <v>1.9184652278177401E-2</v>
       </c>
       <c r="J9" s="2">
@@ -4983,10 +7258,10 @@
       <c r="G10" s="3">
         <v>2.5906735751295299E-3</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="13">
         <v>1.6611295681063099E-3</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <v>3.9968025579536299E-4</v>
       </c>
       <c r="J10" s="3">
@@ -5018,10 +7293,10 @@
       <c r="G11" s="3">
         <v>0.16839378238341901</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <v>0.33970099667774001</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <v>0.24260591526778499</v>
       </c>
       <c r="J11" s="2">
@@ -5053,10 +7328,10 @@
       <c r="G12" s="3">
         <v>0.40025906735751199</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="13">
         <v>0.40199335548172699</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="13">
         <v>0.57793764988009499</v>
       </c>
       <c r="J12" s="2">
@@ -5091,19 +7366,19 @@
         <f t="shared" si="0"/>
         <v>0.99999999999999711</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="13">
         <f t="shared" si="0"/>
         <v>0.99999999999999756</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="13">
         <f t="shared" si="0"/>
         <v>0.99999999999999778</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="13">
         <f t="shared" si="0"/>
         <v>0.99999999999999889</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="13">
         <f t="shared" si="0"/>
         <v>0.99999999999999889</v>
       </c>

</xml_diff>